<commit_message>
top 10 for daging sapi
</commit_message>
<xml_diff>
--- a/Perbandingan_harga_max_Daging_Sapi_2023.xlsx
+++ b/Perbandingan_harga_max_Daging_Sapi_2023.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -565,294 +565,6 @@
         </is>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Riau</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Rp 151.514</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Sumatera Barat</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Rp 145.640</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>DKI Jakarta</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Rp 143.066</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Jambi</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Rp 141.547</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Banten</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Rp 140.562</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Sumatera Selatan</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Rp 139.540</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Jawa Barat</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Rp 138.422</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Sulawesi Tenggara</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Rp 138.111</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Sulawesi Tengah</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Rp 137.352</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>DI Yogyakarta</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Rp 137.311</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Lampung</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>Rp 137.047</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>Bengkulu</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>Rp 136.853</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>Sumatera Utara</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>Rp 136.616</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>Gorontalo</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>Rp 136.267</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>Sulawesi Utara</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>Rp 134.558</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>Jawa Tengah</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>Rp 132.762</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>Maluku Utara</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>Rp 132.023</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>Sulawesi Barat</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>Rp 129.031</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>Sulawesi Selatan</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>Rp 127.397</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>Nusa Tenggara Barat</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>Rp 122.951</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>Maluku</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>Rp 122.080</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>Bali</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>Rp 118.291</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>Jawa Timur</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>Rp 117.427</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>Nusa Tenggara Timur</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>Rp 115.718</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>